<commit_message>
detalles del viaje en proceso
</commit_message>
<xml_diff>
--- a/dev_docs/transportes guerrero/TG - estimacion y .xlsx
+++ b/dev_docs/transportes guerrero/TG - estimacion y .xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <r>
       <t>Proyecto</t>
@@ -55,9 +55,6 @@
     </r>
   </si>
   <si>
-    <t>Tiempo</t>
-  </si>
-  <si>
     <t>Tarea</t>
   </si>
   <si>
@@ -91,15 +88,9 @@
     </r>
   </si>
   <si>
-    <t>crear repositorio</t>
-  </si>
-  <si>
     <t>instalar framework</t>
   </si>
   <si>
-    <t>crear dominio y hosting</t>
-  </si>
-  <si>
     <t>crear catalogo clientes</t>
   </si>
   <si>
@@ -115,7 +106,61 @@
     <t>crear catalogo cajas</t>
   </si>
   <si>
-    <t>configurar git-ftp</t>
+    <t>crear catalogo viajes</t>
+  </si>
+  <si>
+    <t>agregar serie y folio</t>
+  </si>
+  <si>
+    <t>guardar fecha y hora en el mismo registro</t>
+  </si>
+  <si>
+    <t>maquetar maestro</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> agregar detalles</t>
+  </si>
+  <si>
+    <t>crear repositorio, dominio y hosting, instalar git ftp</t>
+  </si>
+  <si>
+    <t>seleccionar caja de manera automatica al seleccionar vehiculo</t>
+  </si>
+  <si>
+    <t>busquedas ajax al combo de clientes</t>
+  </si>
+  <si>
+    <t>busquedas ajax al combo de choferes</t>
+  </si>
+  <si>
+    <t>busquedas ajax al combo de vehiculos</t>
+  </si>
+  <si>
+    <t>actualizar label folio al guardar</t>
+  </si>
+  <si>
+    <t>agregar combo clientes</t>
+  </si>
+  <si>
+    <t>agregar combo choferes</t>
+  </si>
+  <si>
+    <t>agregar combo vehiculos</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>Falta</t>
+  </si>
+  <si>
+    <t>Real</t>
+  </si>
+  <si>
+    <t>Pen.</t>
+  </si>
+  <si>
+    <t>Est</t>
   </si>
 </sst>
 </file>
@@ -218,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -235,6 +280,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -244,10 +290,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,141 +598,351 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.85546875" customWidth="1"/>
-    <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="3" width="8" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="1"/>
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-    </row>
-    <row r="3" spans="1:18" ht="24.75" x14ac:dyDescent="0.4">
+      <c r="L1" s="1"/>
+    </row>
+    <row r="3" spans="1:19" ht="24.75" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <f>SUM(B10:B92)</f>
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E5" s="14">
+        <f>SUM(A10:A49)</f>
+        <v>5.3</v>
+      </c>
+      <c r="F5">
+        <f>SUM(C10:C132)</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <f>SUM(B10:B91)</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="C9" s="8"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>0.5</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0.3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>0.3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0.3</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0.5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0.3</v>
+      </c>
+      <c r="C16">
+        <v>1.5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
+        <f t="shared" ref="A17:A29" si="0">B17</f>
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>0.3</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>0.3</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>0.3</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="14">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="B22">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="B23">
+        <v>0.5</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="14">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:18" ht="18" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="1:18" ht="18" x14ac:dyDescent="0.25">
-      <c r="C11" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="18" x14ac:dyDescent="0.25">
-      <c r="C12" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="18" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>0.5</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>13</v>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="14">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="B25">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="14">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="B26">
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="B27">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="B28">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="B29">
+        <v>0.1</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C10:I10"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="C16:R16"/>
+    <mergeCell ref="D10:J10"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="D14:S14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
primera muestra de avances.
</commit_message>
<xml_diff>
--- a/dev_docs/transportes guerrero/TG - estimacion y .xlsx
+++ b/dev_docs/transportes guerrero/TG - estimacion y .xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Tarea</t>
   </si>
@@ -158,6 +158,18 @@
   </si>
   <si>
     <t>filtros de busqueda</t>
+  </si>
+  <si>
+    <t>provar en navegadores ie, firefox, chrome</t>
+  </si>
+  <si>
+    <t>validar casos de error</t>
+  </si>
+  <si>
+    <t>usar hora de mazatlan en lugar del servidor</t>
+  </si>
+  <si>
+    <t>agregar transaccion para el proceso de guardado del viaje</t>
   </si>
 </sst>
 </file>
@@ -594,9 +606,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -632,7 +644,7 @@
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E4">
         <f>SUM(C10:C104)</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -641,11 +653,11 @@
       </c>
       <c r="D5">
         <f>SUM(B10:B92)</f>
-        <v>10.199999999999999</v>
+        <v>11.7</v>
       </c>
       <c r="E5" s="8">
         <f>D5-E4</f>
-        <v>7.6999999999999993</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="F5" s="8"/>
     </row>
@@ -781,6 +793,9 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
+      <c r="B17">
+        <v>0</v>
+      </c>
       <c r="C17">
         <v>0</v>
       </c>
@@ -887,10 +902,10 @@
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C26">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>17</v>
@@ -899,10 +914,10 @@
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C27">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>18</v>
@@ -911,10 +926,10 @@
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>19</v>
@@ -937,10 +952,54 @@
         <v>0.5</v>
       </c>
       <c r="C30">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>0.5</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>0.5</v>
+      </c>
+      <c r="C32">
+        <v>0.5</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>0.5</v>
+      </c>
+      <c r="C33">
+        <v>0.5</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>0.5</v>
+      </c>
+      <c r="C34">
+        <v>0.5</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
maqueta de la pantalla de consumo
</commit_message>
<xml_diff>
--- a/dev_docs/transportes guerrero/TG - estimacion y .xlsx
+++ b/dev_docs/transportes guerrero/TG - estimacion y .xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>Tarea</t>
   </si>
@@ -177,6 +177,39 @@
   </si>
   <si>
     <t>crear catalogo consumo</t>
+  </si>
+  <si>
+    <t>al seleccionar vehiculo, rellenar la caja rendimiento</t>
+  </si>
+  <si>
+    <t>al modificar distancia o rendimieno actualizar consumo en litros</t>
+  </si>
+  <si>
+    <t>al modificar kilometraje inicial o kilometraje final, actualizar kilometraje recorrido</t>
+  </si>
+  <si>
+    <t>al modificar conumo en litros o precio x litro, actualizar consumo $ y diesel calculado (en el segundo fieldset)</t>
+  </si>
+  <si>
+    <t>implementar calculo de consumo en litros</t>
+  </si>
+  <si>
+    <t>implementar calculo de consumo en pesos</t>
+  </si>
+  <si>
+    <t>implementar calculo de kilometraje recorrido</t>
+  </si>
+  <si>
+    <t>calcular diesel lt</t>
+  </si>
+  <si>
+    <t>calcular diesel pesos</t>
+  </si>
+  <si>
+    <t>mostrar diferenca contra calculado</t>
+  </si>
+  <si>
+    <t>mostrar diferencia contra medido</t>
   </si>
 </sst>
 </file>
@@ -615,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,10 +1057,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,7 +1095,7 @@
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E4">
         <f>SUM(C10:C94)</f>
-        <v>2.8</v>
+        <v>4.1000000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1071,11 +1104,11 @@
       </c>
       <c r="D5">
         <f>SUM(B10:B82)</f>
-        <v>2.1</v>
+        <v>4.4000000000000012</v>
       </c>
       <c r="E5" s="8">
         <f>D5-E4</f>
-        <v>-0.69999999999999973</v>
+        <v>0.30000000000000071</v>
       </c>
       <c r="F5" s="8"/>
     </row>
@@ -1145,10 +1178,10 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>30</v>
@@ -1181,77 +1214,126 @@
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="C19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C22">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C23">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>0.2</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>0.2</v>
+      </c>
+      <c r="C25">
+        <v>0.2</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>0.2</v>
+      </c>
+      <c r="C26">
+        <v>0.2</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
calculos de consumo funcionando
</commit_message>
<xml_diff>
--- a/dev_docs/transportes guerrero/TG - estimacion y .xlsx
+++ b/dev_docs/transportes guerrero/TG - estimacion y .xlsx
@@ -648,7 +648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1060,7 +1060,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
pantalla de gastos basica
</commit_message>
<xml_diff>
--- a/dev_docs/transportes guerrero/TG - estimacion y .xlsx
+++ b/dev_docs/transportes guerrero/TG - estimacion y .xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="16515" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="16515" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
   <si>
     <t>Tarea</t>
   </si>
@@ -211,12 +212,87 @@
   <si>
     <t>mostrar diferencia contra medido</t>
   </si>
+  <si>
+    <t>quiero registrar todos los gastos relacionados con mi negocio y consultarlos de la manera más apropiada.</t>
+  </si>
+  <si>
+    <r>
+      <t>Proyecto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBFBFBF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Escrúpulos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Costo</t>
+  </si>
+  <si>
+    <t>Avance</t>
+  </si>
+  <si>
+    <t>Falta</t>
+  </si>
+  <si>
+    <t>catalogo gastos</t>
+  </si>
+  <si>
+    <t>vista gastos del dia</t>
+  </si>
+  <si>
+    <t>vista gastos historicos</t>
+  </si>
+  <si>
+    <t>catalogo tipos de gasto</t>
+  </si>
+  <si>
+    <t>agregar combo tipo de gasto</t>
+  </si>
+  <si>
+    <t>mostrar el tipo de gasto en la busqueda</t>
+  </si>
+  <si>
+    <t>sincronizar gastos del viajes con los gastos diarios</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +355,13 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -312,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -345,6 +428,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1059,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1344,4 +1429,208 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="3" width="8" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="3" spans="1:13" ht="24.75" x14ac:dyDescent="0.4">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="14">
+        <f>SUM(B11:B78)</f>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="15">
+        <f>D5*500</f>
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="8">
+        <f>D5-E4</f>
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="8">
+        <f>SUM(C11:C82)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="B10" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="L10">
+        <v>0.3</v>
+      </c>
+      <c r="M10">
+        <f>L10*M9/L9</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11">
+        <v>0.3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12">
+        <v>0.2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>0.3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>0.3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18">
+        <v>0.5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19">
+        <v>0.5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="D22" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B10:I10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
seleccion de serie: ON
</commit_message>
<xml_diff>
--- a/dev_docs/transportes guerrero/TG - estimacion y .xlsx
+++ b/dev_docs/transportes guerrero/TG - estimacion y .xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
   <si>
     <t>Tarea</t>
   </si>
@@ -283,6 +283,12 @@
   </si>
   <si>
     <t>sincronizar gastos del viajes con los gastos diarios</t>
+  </si>
+  <si>
+    <t>agregar busqueda ajax al combo tipo gasto</t>
+  </si>
+  <si>
+    <t>mostrar el total de gastos del dia en la pantalla de busqueda</t>
   </si>
 </sst>
 </file>
@@ -413,6 +419,8 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -428,8 +436,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -734,7 +740,7 @@
   <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,13 +752,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -796,22 +802,22 @@
       <c r="C8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="10"/>
+      <c r="D8" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="12"/>
     </row>
     <row r="9" spans="1:19" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
@@ -819,15 +825,15 @@
         <v>1</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
@@ -873,24 +879,24 @@
       <c r="C14">
         <v>0</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="12"/>
-      <c r="S14" s="12"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
@@ -1144,7 +1150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -1157,13 +1163,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1207,22 +1213,22 @@
       <c r="C8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="10"/>
+      <c r="D8" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="12"/>
     </row>
     <row r="9" spans="1:12" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
@@ -1436,7 +1442,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,13 +1454,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1472,16 +1478,16 @@
       <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="9">
         <f>SUM(B11:B78)</f>
-        <v>4.0999999999999996</v>
+        <v>4.7</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="10">
         <f>D5*500</f>
-        <v>2050</v>
+        <v>2350</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1489,8 +1495,8 @@
         <v>49</v>
       </c>
       <c r="D6" s="8">
-        <f>D5-E4</f>
-        <v>4.0999999999999996</v>
+        <f>D5-D7</f>
+        <v>0.60000000000000053</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1499,7 +1505,7 @@
       </c>
       <c r="D7" s="8">
         <f>SUM(C11:C82)</f>
-        <v>0</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1512,10 +1518,10 @@
       <c r="C9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="10"/>
+      <c r="D9" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="12"/>
       <c r="L9">
         <v>1</v>
       </c>
@@ -1523,17 +1529,17 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
+    <row r="10" spans="1:13" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
       <c r="L10">
         <v>0.3</v>
       </c>
@@ -1547,75 +1553,108 @@
       <c r="B11">
         <v>0.3</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
-      <c r="B12">
-        <v>0.2</v>
-      </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13">
+        <v>0.2</v>
+      </c>
+      <c r="C13">
+        <v>0.2</v>
+      </c>
+      <c r="D13" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>0.3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>0.3</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>0.3</v>
+      </c>
+      <c r="C15">
+        <v>0.3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>0.3</v>
+      </c>
+      <c r="C16">
+        <v>0.3</v>
+      </c>
+      <c r="D16" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="7"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
-      <c r="D17" s="7"/>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18">
         <v>0.5</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18">
+        <v>0.5</v>
+      </c>
+      <c r="D18" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19">
         <v>0.5</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19">
+        <v>0.5</v>
+      </c>
+      <c r="D19" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
+      <c r="B20">
+        <v>0.3</v>
+      </c>
+      <c r="C20">
+        <v>0.3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>

</xml_diff>